<commit_message>
Impact site Tab B
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="443" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="443" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -17,15 +17,16 @@
     <sheet name="SIA1" sheetId="5" r:id="rId3"/>
     <sheet name="SIA2" sheetId="6" r:id="rId4"/>
     <sheet name="SIA3" sheetId="7" r:id="rId5"/>
-    <sheet name="Espece X" sheetId="3" r:id="rId6"/>
-    <sheet name="Habitat Y" sheetId="4" r:id="rId7"/>
+    <sheet name="SB" sheetId="8" r:id="rId6"/>
+    <sheet name="Espece X" sheetId="3" r:id="rId7"/>
+    <sheet name="Habitat Y" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="129">
   <si>
     <t>Titre du projet</t>
   </si>
@@ -166,6 +167,252 @@
   </si>
   <si>
     <t>Code SIG OSO</t>
+  </si>
+  <si>
+    <t>Périmètre</t>
+  </si>
+  <si>
+    <t>Critère</t>
+  </si>
+  <si>
+    <t>Indicateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur à l'état initial </t>
+  </si>
+  <si>
+    <t>Périmètre site</t>
+  </si>
+  <si>
+    <t>Diversité habitat</t>
+  </si>
+  <si>
+    <t>Nombre d'habitat forestier</t>
+  </si>
+  <si>
+    <t>Surface (ha) d'habitat forestier</t>
+  </si>
+  <si>
+    <t>Nombre d'habitat ouvert</t>
+  </si>
+  <si>
+    <t>Surface (ha) d'habitat ouvert</t>
+  </si>
+  <si>
+    <t>Nombre d'habitat buissonnant</t>
+  </si>
+  <si>
+    <t>Surface (ha) d'habitat buissonnant</t>
+  </si>
+  <si>
+    <t>Nombre d'habitat rocheux</t>
+  </si>
+  <si>
+    <t>Surface (ha) d'habitat rocheux</t>
+  </si>
+  <si>
+    <t>Nombre de zone humide</t>
+  </si>
+  <si>
+    <t>Surface (ha) de zone humide</t>
+  </si>
+  <si>
+    <t>Nombre d'habitat aquatique</t>
+  </si>
+  <si>
+    <t>Surface (ha) d'habitat aquatique</t>
+  </si>
+  <si>
+    <t>Longueur de lisière (Km) / surface de milieu forestier (Ha)</t>
+  </si>
+  <si>
+    <t>Diversité Espèce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversité avifaune </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversité chiroptères </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversité reptiles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversité amphibiens </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversité mammifères </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversité insectes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversité lépidoptères </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversité odonates </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversité orthoptères </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diversité coléoptères </t>
+  </si>
+  <si>
+    <t>Diversité flore totale</t>
+  </si>
+  <si>
+    <t>Patrimonialité_PS</t>
+  </si>
+  <si>
+    <t>Proportion surfacique des habitat menacés/en danger localement</t>
+  </si>
+  <si>
+    <t>Proportion surfacique des habitat d'intérêt communautaires (et prioritaires)</t>
+  </si>
+  <si>
+    <t>Proportion d'espèces protégées faune au niveau national et regional</t>
+  </si>
+  <si>
+    <t>Proportion d'espèces protégées flore au niveau national et regional</t>
+  </si>
+  <si>
+    <t>Proportion d'espèces menacées faune au niveau national</t>
+  </si>
+  <si>
+    <t>Proportion d'espèces menacées flore au niveau national</t>
+  </si>
+  <si>
+    <t>Proportion d'espèces menacées faune au niveau regional</t>
+  </si>
+  <si>
+    <t>Proportion d'espèces menacées flore au niveau regional</t>
+  </si>
+  <si>
+    <t>Proportion d'espèces faune sur l'annexe II de la DFFH</t>
+  </si>
+  <si>
+    <t>Proportion d'espèces flore sur l'annexe II de la DFFH</t>
+  </si>
+  <si>
+    <t>Proportion d'avifaune sur la DO</t>
+  </si>
+  <si>
+    <t>Fonctionnalité</t>
+  </si>
+  <si>
+    <t>Proportion d'oiseaux nicheurs</t>
+  </si>
+  <si>
+    <t>Proportion d'espèces (hors oiseaux) se reproduisant sur le site</t>
+  </si>
+  <si>
+    <t>Indice de spécialisation de l'avifaune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proportion des chiroptères spécialistes </t>
+  </si>
+  <si>
+    <t>Proportion surfacique des habitats en bon état de conservation</t>
+  </si>
+  <si>
+    <t>Pression_PS</t>
+  </si>
+  <si>
+    <t>% de milieux NON cultivées</t>
+  </si>
+  <si>
+    <t>% de zones NON imperméabilisées</t>
+  </si>
+  <si>
+    <t>Nombre d'espèces d'EEE</t>
+  </si>
+  <si>
+    <t>Nombre de patchs d'EEE</t>
+  </si>
+  <si>
+    <t>% recouvrement des EEE</t>
+  </si>
+  <si>
+    <t>Périmètre élargi</t>
+  </si>
+  <si>
+    <t>Connectivité</t>
+  </si>
+  <si>
+    <t>Longueur de linéaire de transport (Km)</t>
+  </si>
+  <si>
+    <t>Longueur de linéaire de haie (PS et PE)</t>
+  </si>
+  <si>
+    <t>Surface (Ha) de corridor traversant le site</t>
+  </si>
+  <si>
+    <t>Nombre d'espèces de cohérence régional TVB dans PS</t>
+  </si>
+  <si>
+    <t>Représentativité</t>
+  </si>
+  <si>
+    <t>% Habitat forestier PS /PE</t>
+  </si>
+  <si>
+    <t>% Habitat ouvert PS /PE</t>
+  </si>
+  <si>
+    <t>% Habitat buissonnant PS /PE</t>
+  </si>
+  <si>
+    <t>% Habitat rocheux PS /PE</t>
+  </si>
+  <si>
+    <t>% Habitat humide PS /PE</t>
+  </si>
+  <si>
+    <t>% Habitat aquatique PS /PE</t>
+  </si>
+  <si>
+    <t>Patrimonialité_PE</t>
+  </si>
+  <si>
+    <t>Nombre d'espaces protégé ou à enjeu (au mons 1/3 de la surface dans le PE)</t>
+  </si>
+  <si>
+    <t>Nb espèces faune déterminante des Znieffs du PE</t>
+  </si>
+  <si>
+    <t>Nb espèces flore déterminante des Znieffs du PE</t>
+  </si>
+  <si>
+    <t>Pression_PE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milieux cultivés </t>
+  </si>
+  <si>
+    <t>Zones urbanisées</t>
+  </si>
+  <si>
+    <t>Surface d'EEE à proximité immédiate du PS</t>
+  </si>
+  <si>
+    <t>Justification de l'estimation CT</t>
+  </si>
+  <si>
+    <t>Degré d'incertitude CT</t>
+  </si>
+  <si>
+    <t>Valeur après impact CT</t>
+  </si>
+  <si>
+    <t>Justification de l'estimation LT</t>
+  </si>
+  <si>
+    <t>Degré d'incertitude LT</t>
+  </si>
+  <si>
+    <t>Valeur après impact LT</t>
   </si>
 </sst>
 </file>
@@ -796,7 +1043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -826,6 +1073,736 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="153.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="107.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="153.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="107.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" t="s">
+        <v>115</v>
+      </c>
+      <c r="C58" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>102</v>
+      </c>
+      <c r="B59" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>102</v>
+      </c>
+      <c r="B62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -894,7 +1871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>

</xml_diff>

<commit_message>
widget for id of data entry by hand
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -310,9 +310,6 @@
     <t>Indice de spécialisation de l'avifaune</t>
   </si>
   <si>
-    <t xml:space="preserve">Proportion des chiroptères spécialistes </t>
-  </si>
-  <si>
     <t>Proportion surfacique des habitats en bon état de conservation</t>
   </si>
   <si>
@@ -376,9 +373,6 @@
     <t>Patrimonialité_PE</t>
   </si>
   <si>
-    <t>Nombre d'espaces protégé ou à enjeu (au mons 1/3 de la surface dans le PE)</t>
-  </si>
-  <si>
     <t>Nb espèces faune déterminante des Znieffs du PE</t>
   </si>
   <si>
@@ -413,6 +407,12 @@
   </si>
   <si>
     <t>Valeur après impact LT</t>
+  </si>
+  <si>
+    <t>Proportion des chiroptères spécialistes</t>
+  </si>
+  <si>
+    <t>Nombre d'espaces protégé ou à enjeu (au moins 1/3 de la surface dans le PE)</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,22 +1108,22 @@
         <v>50</v>
       </c>
       <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" t="s">
         <v>123</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>124</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>125</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>126</v>
-      </c>
-      <c r="I1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
         <v>90</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1563,7 +1563,7 @@
         <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1571,10 +1571,10 @@
         <v>51</v>
       </c>
       <c r="B42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" t="s">
         <v>96</v>
-      </c>
-      <c r="C42" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1582,10 +1582,10 @@
         <v>51</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1593,10 +1593,10 @@
         <v>51</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1604,10 +1604,10 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1615,186 +1615,186 @@
         <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" t="s">
         <v>102</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>103</v>
-      </c>
-      <c r="C47" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" t="s">
         <v>102</v>
       </c>
-      <c r="B48" t="s">
-        <v>103</v>
-      </c>
       <c r="C48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" t="s">
         <v>102</v>
       </c>
-      <c r="B49" t="s">
-        <v>103</v>
-      </c>
       <c r="C49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" t="s">
         <v>102</v>
       </c>
-      <c r="B50" t="s">
-        <v>103</v>
-      </c>
       <c r="C50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" t="s">
         <v>108</v>
-      </c>
-      <c r="C51" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C57" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" t="s">
         <v>115</v>
-      </c>
-      <c r="C58" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C59" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C60" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" t="s">
         <v>119</v>
-      </c>
-      <c r="C61" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B62" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C62" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add sublists habitat species -> impact site
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="443" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="443" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,10 @@
     <sheet name="SIA1" sheetId="5" r:id="rId3"/>
     <sheet name="SIA2" sheetId="6" r:id="rId4"/>
     <sheet name="SIA3" sheetId="7" r:id="rId5"/>
-    <sheet name="SB" sheetId="8" r:id="rId6"/>
+    <sheet name="SIB" sheetId="8" r:id="rId6"/>
     <sheet name="Espece X" sheetId="3" r:id="rId7"/>
     <sheet name="Habitat Y" sheetId="4" r:id="rId8"/>
+    <sheet name="SIC" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1076,7 +1077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
@@ -1945,4 +1946,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new model tab
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="443" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="443" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="169">
   <si>
     <t>Titre du projet</t>
   </si>
@@ -414,6 +414,126 @@
   </si>
   <si>
     <t>Nombre d'espaces protégé ou à enjeu (au moins 1/3 de la surface dans le PE)</t>
+  </si>
+  <si>
+    <t>Echelle</t>
+  </si>
+  <si>
+    <t>Indicateurs</t>
+  </si>
+  <si>
+    <t>Valeur EI</t>
+  </si>
+  <si>
+    <t>Justification prédiction court terme</t>
+  </si>
+  <si>
+    <t>Incertitudes</t>
+  </si>
+  <si>
+    <t>Valeur après impact/ MC CT</t>
+  </si>
+  <si>
+    <t>Justification prédiction long terme</t>
+  </si>
+  <si>
+    <t>Valeur après impact/ MC LT</t>
+  </si>
+  <si>
+    <t>SITE</t>
+  </si>
+  <si>
+    <t>Diversité espèce</t>
+  </si>
+  <si>
+    <t>Nombre d'espèces dépendantes de l'habitat pour leur cycle de vie (Laisser la possibilité d’ajouter des taxons)</t>
+  </si>
+  <si>
+    <t>Nombre d'espèces flore</t>
+  </si>
+  <si>
+    <t>Surface totale habitat</t>
+  </si>
+  <si>
+    <t>Nombre de patches d'habitat</t>
+  </si>
+  <si>
+    <t>Nombre de micro-habitats</t>
+  </si>
+  <si>
+    <t>Nombre d'horizons de sol par rapport à la référence</t>
+  </si>
+  <si>
+    <t>Epaisseur d'horizons organiques par rapport à la référence</t>
+  </si>
+  <si>
+    <t>Abondance relative de faune détritivore</t>
+  </si>
+  <si>
+    <t>Nombre d'espèces dépendantes de l'habitat pour la reproduction (Laisser la possibilité d’ajouter des taxons)</t>
+  </si>
+  <si>
+    <t>Nombre de Très Gros Bois Vivant</t>
+  </si>
+  <si>
+    <t>Proportion de bois mort</t>
+  </si>
+  <si>
+    <t>Nombre d'espèces bio-indicatrices</t>
+  </si>
+  <si>
+    <t>Densité de lichen</t>
+  </si>
+  <si>
+    <t>Ancienneté de la forêt</t>
+  </si>
+  <si>
+    <t>Nombre d'espèces pollinisatrices</t>
+  </si>
+  <si>
+    <t>Renvoyer vers la méthode sur les fonctionnalités de l'ONEMA</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Proportion de flore dominante</t>
+  </si>
+  <si>
+    <t>Nombre de strates de végétation</t>
+  </si>
+  <si>
+    <t>Hauteur de chaque strate</t>
+  </si>
+  <si>
+    <t>Pression</t>
+  </si>
+  <si>
+    <t>Proportion de sol dégradé</t>
+  </si>
+  <si>
+    <t>Nombre d'espèces indicatrices de pression</t>
+  </si>
+  <si>
+    <t>Temps depuis la dernière coupe</t>
+  </si>
+  <si>
+    <t>Taux de recouvrement des ligneux</t>
+  </si>
+  <si>
+    <t>Taux de couvert des algues dues à l'eutrophisation</t>
+  </si>
+  <si>
+    <t>ELARGI</t>
+  </si>
+  <si>
+    <t>Indice de fragmentation du type d'habitat</t>
+  </si>
+  <si>
+    <t>Surface d'habitat dans le PE</t>
+  </si>
+  <si>
+    <t>% surfacique d'habitat dans le PE</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
@@ -2133,12 +2253,355 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" t="s">
+        <v>159</v>
+      </c>
+      <c r="C22" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
habitat impact site OK
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="170">
   <si>
     <t>Titre du projet</t>
   </si>
@@ -425,18 +425,9 @@
     <t>Valeur EI</t>
   </si>
   <si>
-    <t>Justification prédiction court terme</t>
-  </si>
-  <si>
-    <t>Incertitudes</t>
-  </si>
-  <si>
     <t>Valeur après impact/ MC CT</t>
   </si>
   <si>
-    <t>Justification prédiction long terme</t>
-  </si>
-  <si>
     <t>Valeur après impact/ MC LT</t>
   </si>
   <si>
@@ -534,6 +525,18 @@
   </si>
   <si>
     <t>% surfacique d'habitat dans le PE</t>
+  </si>
+  <si>
+    <t>Incertitudes CT</t>
+  </si>
+  <si>
+    <t>Incertitudes LT</t>
+  </si>
+  <si>
+    <t>Justification prédiction CT</t>
+  </si>
+  <si>
+    <t>Justification prédiction LT</t>
   </si>
 </sst>
 </file>
@@ -2255,8 +2258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2265,10 +2268,10 @@
     <col min="3" max="3" width="99.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2286,319 +2289,319 @@
         <v>131</v>
       </c>
       <c r="E1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" t="s">
         <v>133</v>
-      </c>
-      <c r="G1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I1" t="s">
-        <v>133</v>
-      </c>
-      <c r="J1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
         <v>137</v>
-      </c>
-      <c r="B3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
         <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
         <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
         <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
         <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
         <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
         <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
         <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
         <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B12" t="s">
         <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
         <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B14" t="s">
         <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
         <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s">
         <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B17" t="s">
         <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" t="s">
         <v>155</v>
-      </c>
-      <c r="C20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C21" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C22" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B23" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" t="s">
         <v>159</v>
-      </c>
-      <c r="C23" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B24" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C25" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B26" t="s">
         <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B27" t="s">
         <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B28" t="s">
         <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new sheet Tab D species
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="443" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="443" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="Espece X" sheetId="3" r:id="rId7"/>
     <sheet name="Habitat Y" sheetId="4" r:id="rId8"/>
     <sheet name="SIC" sheetId="9" r:id="rId9"/>
+    <sheet name="SID" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="188">
   <si>
     <t>Titre du projet</t>
   </si>
@@ -537,6 +538,60 @@
   </si>
   <si>
     <t>Justification prédiction LT</t>
+  </si>
+  <si>
+    <t>Surface totale (ha) d'habitat favorable</t>
+  </si>
+  <si>
+    <t>Nombre de patches d'habitat favorable</t>
+  </si>
+  <si>
+    <t>Estimation du nombre d’individus (faune)</t>
+  </si>
+  <si>
+    <t>Surface (ha) de nourrissage favorable</t>
+  </si>
+  <si>
+    <t>Surface (ha) de reproduction favorable</t>
+  </si>
+  <si>
+    <t>Estimation du nombre de couple</t>
+  </si>
+  <si>
+    <t>Surface (ha) de chasse favorable</t>
+  </si>
+  <si>
+    <t>Nombre de gîtes favorables</t>
+  </si>
+  <si>
+    <t>Nombre de mâle chanteurs</t>
+  </si>
+  <si>
+    <t>Nombre de pontes</t>
+  </si>
+  <si>
+    <t>Proportion surfacique de plante(s) hôte(s)</t>
+  </si>
+  <si>
+    <t>Nombre de stations / pieds (selon le type de plante)</t>
+  </si>
+  <si>
+    <t>Nombre d'espèces</t>
+  </si>
+  <si>
+    <t>Nombre de familles</t>
+  </si>
+  <si>
+    <t> Surface de milieu ne générant pas de perturbation</t>
+  </si>
+  <si>
+    <t>Nombre d’observations de l’espèce</t>
+  </si>
+  <si>
+    <t>Surface totale (ha) d'habitat favorable connecté au PS</t>
+  </si>
+  <si>
+    <t>Nombre de zones favorables connectées entre elles grâce au site</t>
   </si>
 </sst>
 </file>
@@ -927,6 +982,285 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
@@ -2258,7 +2592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
factorize + new model
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -9,26 +9,32 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="443" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="634" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Site no. X" sheetId="2" r:id="rId2"/>
-    <sheet name="SIA1" sheetId="5" r:id="rId3"/>
-    <sheet name="SIA2" sheetId="6" r:id="rId4"/>
-    <sheet name="SIA3" sheetId="7" r:id="rId5"/>
-    <sheet name="SIB" sheetId="8" r:id="rId6"/>
-    <sheet name="Espece X" sheetId="3" r:id="rId7"/>
-    <sheet name="Habitat Y" sheetId="4" r:id="rId8"/>
+    <sheet name="Espece X" sheetId="3" r:id="rId3"/>
+    <sheet name="Habitat Y" sheetId="4" r:id="rId4"/>
+    <sheet name="SIA1" sheetId="5" r:id="rId5"/>
+    <sheet name="SIA2" sheetId="6" r:id="rId6"/>
+    <sheet name="SIA3" sheetId="7" r:id="rId7"/>
+    <sheet name="SIB" sheetId="8" r:id="rId8"/>
     <sheet name="SIC" sheetId="9" r:id="rId9"/>
     <sheet name="SID" sheetId="10" r:id="rId10"/>
+    <sheet name="SCA1" sheetId="11" r:id="rId11"/>
+    <sheet name="SCA2" sheetId="12" r:id="rId12"/>
+    <sheet name="SCA3" sheetId="13" r:id="rId13"/>
+    <sheet name="SCB" sheetId="14" r:id="rId14"/>
+    <sheet name="SCC" sheetId="15" r:id="rId15"/>
+    <sheet name="SCD" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="188">
   <si>
     <t>Titre du projet</t>
   </si>
@@ -986,8 +992,1708 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="153.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="107.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="153.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="107.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" t="s">
+        <v>112</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" t="s">
+        <v>114</v>
+      </c>
+      <c r="C57" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" t="s">
+        <v>116</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" t="s">
+        <v>118</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" t="s">
+        <v>119</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,10 +3085,155 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.28515625" style="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="1025" width="10.7109375"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625"/>
+    <col min="2" max="1025" width="10.7109375"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,12 +3282,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,12 +3348,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,12 +3381,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2443,157 +4294,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.28515625" style="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="1025" width="10.7109375"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.140625"/>
-    <col min="2" max="1025" width="10.7109375"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bug fix change type of site
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="634" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="741" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Site no. X" sheetId="2" r:id="rId2"/>
     <sheet name="Espece X" sheetId="3" r:id="rId3"/>
     <sheet name="Habitat Y" sheetId="4" r:id="rId4"/>
-    <sheet name="Entree des donnees 1" sheetId="6" r:id="rId5"/>
-    <sheet name="Entree des donnees 2" sheetId="7" r:id="rId6"/>
-    <sheet name="Entree des donnees 3" sheetId="5" r:id="rId7"/>
+    <sheet name="Entree des donnees 1" sheetId="5" r:id="rId5"/>
+    <sheet name="Entree des donnees 2" sheetId="6" r:id="rId6"/>
+    <sheet name="Entree des donnees 3" sheetId="7" r:id="rId7"/>
     <sheet name="Niveau general" sheetId="8" r:id="rId8"/>
     <sheet name="Niveau habitat" sheetId="9" r:id="rId9"/>
     <sheet name="Niveau espece" sheetId="10" r:id="rId10"/>
@@ -1461,7 +1461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1543,10 +1543,64 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,12 +1661,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,60 +1687,6 @@
       </c>
       <c r="D1" t="s">
         <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add '%' text input
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="741" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="741" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -384,12 +384,6 @@
     <t>Pression_PE</t>
   </si>
   <si>
-    <t xml:space="preserve">Milieux cultivés </t>
-  </si>
-  <si>
-    <t>Zones urbanisées</t>
-  </si>
-  <si>
     <t>Surface d'EEE à proximité immédiate du PS</t>
   </si>
   <si>
@@ -595,6 +589,12 @@
   </si>
   <si>
     <t>Appartenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Milieux cultivés </t>
+  </si>
+  <si>
+    <t>% Zones urbanisées</t>
   </si>
 </sst>
 </file>
@@ -990,7 +990,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,254 +1009,254 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s">
         <v>48</v>
       </c>
       <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" t="s">
         <v>130</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" t="s">
         <v>131</v>
-      </c>
-      <c r="E1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I1" t="s">
-        <v>167</v>
-      </c>
-      <c r="J1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
         <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
         <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
         <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
         <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
         <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
         <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
         <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
         <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s">
         <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
         <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
         <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
         <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
         <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B18" t="s">
         <v>107</v>
       </c>
       <c r="C18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B19" t="s">
         <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B20" t="s">
         <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B21" t="s">
         <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -1665,7 +1665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
@@ -1698,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,22 +1730,22 @@
         <v>50</v>
       </c>
       <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" t="s">
         <v>121</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>122</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>123</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>124</v>
-      </c>
-      <c r="I1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2288,7 +2288,7 @@
         <v>90</v>
       </c>
       <c r="C40" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -2526,7 +2526,7 @@
         <v>114</v>
       </c>
       <c r="C57" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2568,7 +2568,7 @@
         <v>117</v>
       </c>
       <c r="C60" t="s">
-        <v>118</v>
+        <v>187</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2582,7 +2582,7 @@
         <v>117</v>
       </c>
       <c r="C61" t="s">
-        <v>119</v>
+        <v>188</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2596,7 +2596,7 @@
         <v>117</v>
       </c>
       <c r="C62" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2611,8 +2611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2630,331 +2630,331 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s">
         <v>48</v>
       </c>
       <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" t="s">
         <v>130</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" t="s">
         <v>131</v>
-      </c>
-      <c r="E1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I1" t="s">
-        <v>167</v>
-      </c>
-      <c r="J1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
         <v>134</v>
-      </c>
-      <c r="B2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" t="s">
         <v>135</v>
-      </c>
-      <c r="C3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
         <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
         <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
         <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
         <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
         <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
         <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s">
         <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
         <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
         <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
         <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
         <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
         <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
         <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
         <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19" t="s">
         <v>152</v>
-      </c>
-      <c r="C19" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C21" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" t="s">
         <v>156</v>
-      </c>
-      <c r="C22" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B26" t="s">
         <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B27" t="s">
         <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B28" t="s">
         <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new tab for the justification of the initial states
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabricezaoui/Codes/ECOVAL/model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabrice/Applications/Codes/ECOVAL/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33110A71-6B39-AD48-B2E1-0AB92E5AEE6B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE42560-8B81-0D41-B75E-437DD4E3640B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7280" yWindow="3520" windowWidth="33200" windowHeight="20660" tabRatio="741" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="188">
   <si>
     <t>Titre du projet</t>
   </si>
@@ -590,6 +590,9 @@
   </si>
   <si>
     <t>Elargi</t>
+  </si>
+  <si>
+    <t>Justification</t>
   </si>
 </sst>
 </file>
@@ -982,10 +985,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -994,15 +997,16 @@
     <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>125</v>
       </c>
@@ -1016,25 +1020,28 @@
         <v>127</v>
       </c>
       <c r="E1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s">
         <v>162</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>160</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>128</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>163</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>161</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -1045,7 +1052,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>185</v>
       </c>
@@ -1056,7 +1063,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>185</v>
       </c>
@@ -1067,7 +1074,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>185</v>
       </c>
@@ -1078,7 +1085,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>185</v>
       </c>
@@ -1089,7 +1096,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>185</v>
       </c>
@@ -1100,7 +1107,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>185</v>
       </c>
@@ -1111,7 +1118,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>185</v>
       </c>
@@ -1122,7 +1129,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>185</v>
       </c>
@@ -1133,7 +1140,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>185</v>
       </c>
@@ -1144,7 +1151,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>185</v>
       </c>
@@ -1155,7 +1162,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>185</v>
       </c>
@@ -1166,7 +1173,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>185</v>
       </c>
@@ -1177,7 +1184,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>185</v>
       </c>
@@ -1188,7 +1195,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>185</v>
       </c>
@@ -2604,10 +2611,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2615,15 +2622,16 @@
     <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="99.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>125</v>
       </c>
@@ -2637,25 +2645,28 @@
         <v>127</v>
       </c>
       <c r="E1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s">
         <v>162</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>160</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>128</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>163</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>161</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -2666,7 +2677,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>185</v>
       </c>
@@ -2677,7 +2688,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>185</v>
       </c>
@@ -2688,7 +2699,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>185</v>
       </c>
@@ -2699,7 +2710,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>185</v>
       </c>
@@ -2710,7 +2721,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>185</v>
       </c>
@@ -2721,7 +2732,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>185</v>
       </c>
@@ -2732,7 +2743,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>185</v>
       </c>
@@ -2743,7 +2754,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>185</v>
       </c>
@@ -2754,7 +2765,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>185</v>
       </c>
@@ -2765,7 +2776,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>185</v>
       </c>
@@ -2776,7 +2787,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>185</v>
       </c>
@@ -2787,7 +2798,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>185</v>
       </c>
@@ -2798,7 +2809,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>185</v>
       </c>
@@ -2809,7 +2820,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>185</v>
       </c>

</xml_diff>

<commit_message>
delete one row 'Niveau Espèce'
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="186">
   <si>
     <t>Titre du projet</t>
   </si>
@@ -978,10 +978,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1130,7 @@
         <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1141,7 +1141,7 @@
         <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1152,7 +1152,7 @@
         <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1171,10 +1171,10 @@
         <v>181</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1185,7 +1185,7 @@
         <v>130</v>
       </c>
       <c r="C15" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1193,21 +1193,21 @@
         <v>181</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1218,7 +1218,7 @@
         <v>105</v>
       </c>
       <c r="C18" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1226,10 +1226,10 @@
         <v>182</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1240,17 +1240,6 @@
         <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>182</v>
-      </c>
-      <c r="B21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" t="s">
         <v>177</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- add perimeter values - title changes
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabricezaoui/Codes/ECOVAL/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D91AC0-4091-C54E-BFF1-6BD2E2294417}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="3525" windowWidth="33195" windowHeight="20655" tabRatio="741" activeTab="9"/>
+    <workbookView xWindow="2160" yWindow="740" windowWidth="33200" windowHeight="20660" tabRatio="741" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="187">
   <si>
     <t>Titre du projet</t>
   </si>
@@ -586,12 +587,15 @@
   </si>
   <si>
     <t>Nombre d'espèces dépendantes de l'habitat pour leur cycle de vie</t>
+  </si>
+  <si>
+    <t>Perimetre elargi (km)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -909,20 +913,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.42578125"/>
-    <col min="2" max="1025" width="10.7109375"/>
+    <col min="1" max="1" width="17.5"/>
+    <col min="2" max="1025" width="10.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -930,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -938,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -946,7 +950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -954,7 +958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -962,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -977,29 +981,29 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>125</v>
       </c>
@@ -1034,7 +1038,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>181</v>
       </c>
@@ -1045,7 +1049,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -1056,7 +1060,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>181</v>
       </c>
@@ -1067,7 +1071,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -1078,7 +1082,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>181</v>
       </c>
@@ -1089,7 +1093,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>181</v>
       </c>
@@ -1100,7 +1104,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -1111,7 +1115,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>181</v>
       </c>
@@ -1122,7 +1126,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>181</v>
       </c>
@@ -1133,7 +1137,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>181</v>
       </c>
@@ -1144,7 +1148,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>181</v>
       </c>
@@ -1155,7 +1159,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>181</v>
       </c>
@@ -1166,7 +1170,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>181</v>
       </c>
@@ -1177,7 +1181,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>181</v>
       </c>
@@ -1188,7 +1192,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -1199,7 +1203,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>182</v>
       </c>
@@ -1210,7 +1214,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>182</v>
       </c>
@@ -1221,7 +1225,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>182</v>
       </c>
@@ -1232,7 +1236,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>182</v>
       </c>
@@ -1249,20 +1253,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875"/>
-    <col min="2" max="1025" width="10.7109375"/>
+    <col min="1" max="1" width="17.83203125"/>
+    <col min="2" max="1025" width="10.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1270,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1278,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1286,7 +1290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1294,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1302,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1310,7 +1314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1318,7 +1322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1326,7 +1330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1334,7 +1338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1342,7 +1346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1350,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1365,21 +1369,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" style="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="1025" width="10.7109375"/>
+    <col min="1" max="1" width="33.33203125" style="1"/>
+    <col min="2" max="2" width="11.5" style="1"/>
+    <col min="3" max="1025" width="10.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -1387,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1395,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1403,7 +1407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1411,7 +1415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1419,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1427,11 +1431,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>178</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1442,20 +1454,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625"/>
-    <col min="2" max="1025" width="10.7109375"/>
+    <col min="1" max="1" width="26.1640625"/>
+    <col min="2" max="1025" width="10.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1463,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1471,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1479,7 +1491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1487,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1495,7 +1507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1503,7 +1515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1511,11 +1523,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>178</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1526,26 +1546,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1580,26 +1600,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1646,20 +1666,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1679,28 +1699,28 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A47" sqref="A47:A62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="153.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="107.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="153.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="107.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="153.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="107.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="153.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="107.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1732,7 +1752,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>181</v>
       </c>
@@ -1746,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -1760,7 +1780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>181</v>
       </c>
@@ -1774,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -1788,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>181</v>
       </c>
@@ -1802,7 +1822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>181</v>
       </c>
@@ -1816,7 +1836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -1830,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>181</v>
       </c>
@@ -1844,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>181</v>
       </c>
@@ -1858,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>181</v>
       </c>
@@ -1872,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>181</v>
       </c>
@@ -1886,7 +1906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>181</v>
       </c>
@@ -1900,7 +1920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>181</v>
       </c>
@@ -1914,7 +1934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>181</v>
       </c>
@@ -1928,7 +1948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -1942,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>181</v>
       </c>
@@ -1956,7 +1976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>181</v>
       </c>
@@ -1970,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>181</v>
       </c>
@@ -1984,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>181</v>
       </c>
@@ -1998,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>181</v>
       </c>
@@ -2012,7 +2032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>181</v>
       </c>
@@ -2026,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>181</v>
       </c>
@@ -2040,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>181</v>
       </c>
@@ -2054,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>181</v>
       </c>
@@ -2068,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>181</v>
       </c>
@@ -2082,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>181</v>
       </c>
@@ -2096,7 +2116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>181</v>
       </c>
@@ -2110,7 +2130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>181</v>
       </c>
@@ -2124,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>181</v>
       </c>
@@ -2138,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>181</v>
       </c>
@@ -2152,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>181</v>
       </c>
@@ -2166,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>181</v>
       </c>
@@ -2180,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>181</v>
       </c>
@@ -2194,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>181</v>
       </c>
@@ -2208,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>181</v>
       </c>
@@ -2222,7 +2242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>181</v>
       </c>
@@ -2236,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>181</v>
       </c>
@@ -2250,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>181</v>
       </c>
@@ -2264,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>181</v>
       </c>
@@ -2278,7 +2298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>181</v>
       </c>
@@ -2292,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>181</v>
       </c>
@@ -2306,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>181</v>
       </c>
@@ -2320,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>181</v>
       </c>
@@ -2334,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>181</v>
       </c>
@@ -2348,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>181</v>
       </c>
@@ -2362,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>182</v>
       </c>
@@ -2376,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>182</v>
       </c>
@@ -2390,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>182</v>
       </c>
@@ -2404,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>182</v>
       </c>
@@ -2418,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>182</v>
       </c>
@@ -2432,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>182</v>
       </c>
@@ -2446,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>182</v>
       </c>
@@ -2460,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>182</v>
       </c>
@@ -2474,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>182</v>
       </c>
@@ -2488,7 +2508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>182</v>
       </c>
@@ -2502,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>182</v>
       </c>
@@ -2516,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>182</v>
       </c>
@@ -2530,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>182</v>
       </c>
@@ -2544,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>182</v>
       </c>
@@ -2558,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>182</v>
       </c>
@@ -2572,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>182</v>
       </c>
@@ -2592,28 +2612,28 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="99.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>125</v>
       </c>
@@ -2648,7 +2668,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>181</v>
       </c>
@@ -2659,7 +2679,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -2670,7 +2690,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>181</v>
       </c>
@@ -2681,7 +2701,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -2692,7 +2712,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>181</v>
       </c>
@@ -2703,7 +2723,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>181</v>
       </c>
@@ -2714,7 +2734,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -2725,7 +2745,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>181</v>
       </c>
@@ -2736,7 +2756,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>181</v>
       </c>
@@ -2747,7 +2767,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>181</v>
       </c>
@@ -2758,7 +2778,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>181</v>
       </c>
@@ -2769,7 +2789,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>181</v>
       </c>
@@ -2780,7 +2800,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>181</v>
       </c>
@@ -2791,7 +2811,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>181</v>
       </c>
@@ -2802,7 +2822,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -2813,7 +2833,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>181</v>
       </c>
@@ -2824,7 +2844,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>181</v>
       </c>
@@ -2835,7 +2855,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>181</v>
       </c>
@@ -2846,7 +2866,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>181</v>
       </c>
@@ -2857,7 +2877,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>181</v>
       </c>
@@ -2868,7 +2888,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>181</v>
       </c>
@@ -2879,7 +2899,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>181</v>
       </c>
@@ -2890,7 +2910,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>181</v>
       </c>
@@ -2901,7 +2921,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>182</v>
       </c>
@@ -2912,7 +2932,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>182</v>
       </c>
@@ -2923,7 +2943,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>182</v>
       </c>

</xml_diff>

<commit_message>
a new color and new selections for default initial values
</commit_message>
<xml_diff>
--- a/model/ECOVAL.xlsx
+++ b/model/ECOVAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabricezaoui/Codes/ECOVAL/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D91AC0-4091-C54E-BFF1-6BD2E2294417}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEABC1A-EC42-764D-954C-381EAE470521}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="740" windowWidth="33200" windowHeight="20660" tabRatio="741" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="741" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -229,36 +229,6 @@
     <t>Diversité Espèce</t>
   </si>
   <si>
-    <t xml:space="preserve">Diversité avifaune </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversité chiroptères </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversité reptiles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversité amphibiens </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversité mammifères </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversité insectes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversité lépidoptères </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversité odonates </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversité orthoptères </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diversité coléoptères </t>
-  </si>
-  <si>
     <t>Diversité flore totale</t>
   </si>
   <si>
@@ -568,9 +538,6 @@
     <t>Appartenance</t>
   </si>
   <si>
-    <t xml:space="preserve">% Milieux cultivés </t>
-  </si>
-  <si>
     <t>% Zones urbanisées</t>
   </si>
   <si>
@@ -590,6 +557,39 @@
   </si>
   <si>
     <t>Perimetre elargi (km)</t>
+  </si>
+  <si>
+    <t>Diversité avifaune</t>
+  </si>
+  <si>
+    <t>Diversité chiroptères</t>
+  </si>
+  <si>
+    <t>Diversité reptiles</t>
+  </si>
+  <si>
+    <t>Diversité amphibiens</t>
+  </si>
+  <si>
+    <t>Diversité mammifères</t>
+  </si>
+  <si>
+    <t>Diversité insectes</t>
+  </si>
+  <si>
+    <t>Diversité lépidoptères</t>
+  </si>
+  <si>
+    <t>Diversité odonates</t>
+  </si>
+  <si>
+    <t>Diversité orthoptères</t>
+  </si>
+  <si>
+    <t>Diversité coléoptères</t>
+  </si>
+  <si>
+    <t>% Milieux cultivés</t>
   </si>
 </sst>
 </file>
@@ -1005,246 +1005,246 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
         <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="E1" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="H1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="I1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="J1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="K1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -1457,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -1702,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:A62"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1734,27 +1734,27 @@
         <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="H1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="I1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="J1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
@@ -1768,7 +1768,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
         <v>51</v>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
@@ -1852,7 +1852,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B10" t="s">
         <v>51</v>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
@@ -1894,7 +1894,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B12" t="s">
         <v>51</v>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s">
         <v>51</v>
@@ -1922,7 +1922,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s">
         <v>51</v>
@@ -1936,13 +1936,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B15" t="s">
         <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>176</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1950,13 +1950,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B16" t="s">
         <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>177</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1964,13 +1964,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
         <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>178</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1978,13 +1978,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B18" t="s">
         <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>179</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1992,13 +1992,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B19" t="s">
         <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>180</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2006,13 +2006,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
         <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>181</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2020,13 +2020,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B21" t="s">
         <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>182</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2034,13 +2034,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B22" t="s">
         <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>183</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2048,13 +2048,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>184</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2062,13 +2062,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B24" t="s">
         <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>185</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2076,13 +2076,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B25" t="s">
         <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2090,13 +2090,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2104,13 +2104,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -2118,13 +2118,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2132,13 +2132,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2146,13 +2146,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2160,13 +2160,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2174,13 +2174,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2188,13 +2188,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2202,13 +2202,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2216,13 +2216,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" t="s">
         <v>77</v>
-      </c>
-      <c r="C35" t="s">
-        <v>87</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2230,13 +2230,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2244,13 +2244,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C37" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2258,13 +2258,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2272,13 +2272,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2286,13 +2286,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -2300,13 +2300,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2314,13 +2314,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2328,13 +2328,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C43" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -2342,13 +2342,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C44" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -2356,13 +2356,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -2370,13 +2370,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C46" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2384,13 +2384,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -2398,13 +2398,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C48" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -2412,13 +2412,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B49" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C49" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2426,13 +2426,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C50" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -2440,13 +2440,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B51" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C51" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -2454,13 +2454,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B52" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2468,13 +2468,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -2482,13 +2482,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B54" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C54" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -2496,13 +2496,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C55" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2510,13 +2510,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2524,13 +2524,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B57" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C57" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2538,13 +2538,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B58" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C58" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -2552,13 +2552,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B59" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C59" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2566,13 +2566,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C60" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2580,13 +2580,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B61" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C61" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2594,13 +2594,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B62" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C62" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2635,323 +2635,323 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
         <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="E1" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="G1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="H1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="I1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="J1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="K1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C24" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>